<commit_message>
modification de la taille des images
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cloe-\Documents\OpenClassroom\Projet 4\CloeBlanchard_4_12042021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F61CE8-91A6-40E8-B85B-35F8BBA2B849}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0998F8A-0F0F-474D-BDC4-550A8AB60318}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29850" yWindow="-120" windowWidth="27870" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="89">
   <si>
     <t>Catégorie</t>
   </si>
@@ -263,27 +263,7 @@
     <t>enlever les caractère indésirables</t>
   </si>
   <si>
-    <t>class et id dans la même div</t>
-  </si>
-  <si>
-    <t>Les class et les id sont présent dans la même
- div</t>
-  </si>
-  <si>
-    <t>remplacer l'id par la class</t>
-  </si>
-  <si>
     <t>remettre en ordre les balises titres</t>
-  </si>
-  <si>
-    <t>nom des class et id</t>
-  </si>
-  <si>
-    <t>les noms des class et des ids ne sont pas cohérent avec le sujet</t>
-  </si>
-  <si>
-    <t>remplacer certains noms d'ids et de 
-classes</t>
   </si>
   <si>
     <t>balise sans texte</t>
@@ -331,17 +311,7 @@
  les mêmes sur les deux pages</t>
   </si>
   <si>
-    <t>alt avant src</t>
-  </si>
-  <si>
-    <t>Dans certaines balise img, l'alt est placée 
-avant le src</t>
-  </si>
-  <si>
     <t>remplacer les liens faux</t>
-  </si>
-  <si>
-    <t>Rétablir l'ordre des liens</t>
   </si>
   <si>
     <t>langue html</t>
@@ -358,6 +328,9 @@
   </si>
   <si>
     <t>balises titres manquant</t>
+  </si>
+  <si>
+    <t>mauvaise pratique html</t>
   </si>
 </sst>
 </file>
@@ -673,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1081,21 +1054,11 @@
       <c r="F21" s="7"/>
     </row>
     <row r="22" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="A22" s="6"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
       <c r="F22" s="7"/>
     </row>
     <row r="23" spans="1:6" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1103,13 +1066,13 @@
         <v>7</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>55</v>
@@ -1117,35 +1080,25 @@
       <c r="F23" s="7"/>
     </row>
     <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="A24" s="6"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="7"/>
       <c r="F24" s="7"/>
     </row>
     <row r="25" spans="1:6" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>55</v>
@@ -1157,13 +1110,13 @@
         <v>7</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>55</v>
@@ -1175,13 +1128,13 @@
         <v>11</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>55</v>
@@ -1193,13 +1146,13 @@
         <v>7</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>55</v>
@@ -1211,13 +1164,13 @@
         <v>7</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>55</v>
@@ -1225,21 +1178,11 @@
       <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:6" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="A30" s="6"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
       <c r="F30" s="7"/>
     </row>
     <row r="31" spans="1:6" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1247,13 +1190,13 @@
         <v>7</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>55</v>

</xml_diff>